<commit_message>
update December 07, 2023
</commit_message>
<xml_diff>
--- a/Gradus_QNR_KSE_Discounting_26092023.xlsx
+++ b/Gradus_QNR_KSE_Discounting_26092023.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KSE\Projects\ukraine_discounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58559ADD-AF87-4EA5-8401-703BE62A2018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C747C4CB-4ED3-4FF5-B596-A5C9915ACBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F24B5D40-2C39-44B4-B366-2105998D9FFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F24B5D40-2C39-44B4-B366-2105998D9FFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Brik" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="466">
   <si>
     <t>single</t>
   </si>
@@ -4812,9 +4813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C899D0-6DCF-48AD-A011-F8380857F754}">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C265"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C87:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8196,9 +8197,9 @@
     <cfRule type="duplicateValues" dxfId="271" priority="597"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A7">
-    <cfRule type="duplicateValues" dxfId="270" priority="599"/>
-    <cfRule type="duplicateValues" dxfId="269" priority="590"/>
-    <cfRule type="duplicateValues" dxfId="268" priority="591"/>
+    <cfRule type="duplicateValues" dxfId="270" priority="590"/>
+    <cfRule type="duplicateValues" dxfId="269" priority="591"/>
+    <cfRule type="duplicateValues" dxfId="268" priority="599"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
     <cfRule type="duplicateValues" dxfId="267" priority="596"/>
@@ -8207,102 +8208,102 @@
     <cfRule type="duplicateValues" dxfId="266" priority="592"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="265" priority="594"/>
-    <cfRule type="duplicateValues" dxfId="264" priority="595"/>
-    <cfRule type="duplicateValues" dxfId="263" priority="593"/>
+    <cfRule type="duplicateValues" dxfId="265" priority="593"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="594"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="595"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="262" priority="873"/>
-    <cfRule type="duplicateValues" dxfId="261" priority="872"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="872"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="873"/>
     <cfRule type="duplicateValues" dxfId="260" priority="874"/>
-    <cfRule type="duplicateValues" dxfId="259" priority="876"/>
-    <cfRule type="duplicateValues" dxfId="258" priority="875"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="875"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="876"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A35">
-    <cfRule type="duplicateValues" dxfId="257" priority="655"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="653"/>
     <cfRule type="duplicateValues" dxfId="256" priority="654"/>
-    <cfRule type="duplicateValues" dxfId="255" priority="653"/>
+    <cfRule type="duplicateValues" dxfId="255" priority="655"/>
     <cfRule type="duplicateValues" dxfId="254" priority="656"/>
     <cfRule type="duplicateValues" dxfId="253" priority="657"/>
     <cfRule type="duplicateValues" dxfId="252" priority="658"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="251" priority="652"/>
-    <cfRule type="duplicateValues" dxfId="250" priority="651"/>
-    <cfRule type="duplicateValues" dxfId="249" priority="650"/>
-    <cfRule type="duplicateValues" dxfId="248" priority="649"/>
-    <cfRule type="duplicateValues" dxfId="247" priority="648"/>
-    <cfRule type="duplicateValues" dxfId="246" priority="647"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="647"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="648"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="649"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="650"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="651"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="652"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
     <cfRule type="duplicateValues" dxfId="245" priority="240"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:A38">
-    <cfRule type="duplicateValues" dxfId="244" priority="239"/>
-    <cfRule type="duplicateValues" dxfId="243" priority="242"/>
-    <cfRule type="duplicateValues" dxfId="242" priority="243"/>
-    <cfRule type="duplicateValues" dxfId="241" priority="244"/>
-    <cfRule type="duplicateValues" dxfId="240" priority="245"/>
-    <cfRule type="duplicateValues" dxfId="239" priority="246"/>
-    <cfRule type="duplicateValues" dxfId="238" priority="247"/>
-    <cfRule type="duplicateValues" dxfId="237" priority="234"/>
-    <cfRule type="duplicateValues" dxfId="236" priority="233"/>
-    <cfRule type="duplicateValues" dxfId="235" priority="235"/>
-    <cfRule type="duplicateValues" dxfId="234" priority="236"/>
-    <cfRule type="duplicateValues" dxfId="233" priority="237"/>
-    <cfRule type="duplicateValues" dxfId="232" priority="238"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="233"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="234"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="235"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="236"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="238"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="239"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="242"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="243"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="244"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="245"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="246"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="247"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
     <cfRule type="duplicateValues" dxfId="231" priority="241"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="duplicateValues" dxfId="230" priority="863"/>
-    <cfRule type="duplicateValues" dxfId="229" priority="864"/>
-    <cfRule type="duplicateValues" dxfId="228" priority="865"/>
-    <cfRule type="duplicateValues" dxfId="227" priority="866"/>
-    <cfRule type="duplicateValues" dxfId="226" priority="862"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="862"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="863"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="864"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="865"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="866"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
     <cfRule type="duplicateValues" dxfId="225" priority="857"/>
     <cfRule type="duplicateValues" dxfId="224" priority="858"/>
-    <cfRule type="duplicateValues" dxfId="223" priority="860"/>
-    <cfRule type="duplicateValues" dxfId="222" priority="861"/>
-    <cfRule type="duplicateValues" dxfId="221" priority="859"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="859"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="860"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="861"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="duplicateValues" dxfId="220" priority="853"/>
-    <cfRule type="duplicateValues" dxfId="219" priority="852"/>
-    <cfRule type="duplicateValues" dxfId="218" priority="855"/>
-    <cfRule type="duplicateValues" dxfId="217" priority="854"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="852"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="853"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="854"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="855"/>
     <cfRule type="duplicateValues" dxfId="216" priority="856"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A72">
-    <cfRule type="duplicateValues" dxfId="215" priority="626"/>
-    <cfRule type="duplicateValues" dxfId="214" priority="627"/>
-    <cfRule type="duplicateValues" dxfId="213" priority="628"/>
-    <cfRule type="duplicateValues" dxfId="212" priority="629"/>
-    <cfRule type="duplicateValues" dxfId="211" priority="630"/>
-    <cfRule type="duplicateValues" dxfId="210" priority="625"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="625"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="626"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="627"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="628"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="629"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="630"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73">
-    <cfRule type="duplicateValues" dxfId="209" priority="925"/>
-    <cfRule type="duplicateValues" dxfId="208" priority="924"/>
-    <cfRule type="duplicateValues" dxfId="207" priority="923"/>
-    <cfRule type="duplicateValues" dxfId="206" priority="922"/>
-    <cfRule type="duplicateValues" dxfId="205" priority="921"/>
-    <cfRule type="duplicateValues" dxfId="204" priority="920"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="920"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="921"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="922"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="923"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="924"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="925"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74">
     <cfRule type="duplicateValues" dxfId="203" priority="149"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:A75">
-    <cfRule type="duplicateValues" dxfId="202" priority="143"/>
-    <cfRule type="duplicateValues" dxfId="201" priority="144"/>
-    <cfRule type="duplicateValues" dxfId="200" priority="145"/>
-    <cfRule type="duplicateValues" dxfId="199" priority="146"/>
-    <cfRule type="duplicateValues" dxfId="198" priority="147"/>
-    <cfRule type="duplicateValues" dxfId="197" priority="148"/>
-    <cfRule type="duplicateValues" dxfId="196" priority="142"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="142"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="143"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="144"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="145"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="146"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="147"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="148"/>
     <cfRule type="duplicateValues" dxfId="195" priority="151"/>
     <cfRule type="duplicateValues" dxfId="194" priority="152"/>
     <cfRule type="duplicateValues" dxfId="193" priority="153"/>
@@ -8314,86 +8315,86 @@
     <cfRule type="duplicateValues" dxfId="189" priority="150"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76">
-    <cfRule type="duplicateValues" dxfId="188" priority="850"/>
-    <cfRule type="duplicateValues" dxfId="187" priority="851"/>
-    <cfRule type="duplicateValues" dxfId="186" priority="847"/>
-    <cfRule type="duplicateValues" dxfId="185" priority="848"/>
-    <cfRule type="duplicateValues" dxfId="184" priority="849"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="847"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="848"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="849"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="850"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="851"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="duplicateValues" dxfId="183" priority="844"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="842"/>
     <cfRule type="duplicateValues" dxfId="182" priority="843"/>
-    <cfRule type="duplicateValues" dxfId="181" priority="842"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="844"/>
     <cfRule type="duplicateValues" dxfId="180" priority="845"/>
     <cfRule type="duplicateValues" dxfId="179" priority="846"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="duplicateValues" dxfId="178" priority="836"/>
-    <cfRule type="duplicateValues" dxfId="177" priority="835"/>
-    <cfRule type="duplicateValues" dxfId="176" priority="833"/>
-    <cfRule type="duplicateValues" dxfId="175" priority="832"/>
-    <cfRule type="duplicateValues" dxfId="174" priority="834"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="832"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="833"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="834"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="835"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="836"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="duplicateValues" dxfId="173" priority="831"/>
-    <cfRule type="duplicateValues" dxfId="172" priority="830"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="827"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="828"/>
     <cfRule type="duplicateValues" dxfId="171" priority="829"/>
-    <cfRule type="duplicateValues" dxfId="170" priority="828"/>
-    <cfRule type="duplicateValues" dxfId="169" priority="827"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="830"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="831"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="duplicateValues" dxfId="168" priority="826"/>
-    <cfRule type="duplicateValues" dxfId="167" priority="825"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="822"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="823"/>
     <cfRule type="duplicateValues" dxfId="166" priority="824"/>
-    <cfRule type="duplicateValues" dxfId="165" priority="823"/>
-    <cfRule type="duplicateValues" dxfId="164" priority="822"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="825"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="826"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="duplicateValues" dxfId="163" priority="820"/>
-    <cfRule type="duplicateValues" dxfId="162" priority="817"/>
-    <cfRule type="duplicateValues" dxfId="161" priority="818"/>
-    <cfRule type="duplicateValues" dxfId="160" priority="819"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="817"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="818"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="819"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="820"/>
     <cfRule type="duplicateValues" dxfId="159" priority="821"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="duplicateValues" dxfId="158" priority="814"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="812"/>
     <cfRule type="duplicateValues" dxfId="157" priority="813"/>
-    <cfRule type="duplicateValues" dxfId="156" priority="812"/>
-    <cfRule type="duplicateValues" dxfId="155" priority="816"/>
-    <cfRule type="duplicateValues" dxfId="154" priority="815"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="814"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="815"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="816"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="duplicateValues" dxfId="153" priority="809"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="807"/>
     <cfRule type="duplicateValues" dxfId="152" priority="808"/>
-    <cfRule type="duplicateValues" dxfId="151" priority="807"/>
-    <cfRule type="duplicateValues" dxfId="150" priority="811"/>
-    <cfRule type="duplicateValues" dxfId="149" priority="810"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="809"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="810"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="811"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="duplicateValues" dxfId="148" priority="805"/>
-    <cfRule type="duplicateValues" dxfId="147" priority="804"/>
-    <cfRule type="duplicateValues" dxfId="146" priority="803"/>
-    <cfRule type="duplicateValues" dxfId="145" priority="806"/>
-    <cfRule type="duplicateValues" dxfId="144" priority="802"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="802"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="803"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="804"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="805"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="806"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="duplicateValues" dxfId="143" priority="799"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="797"/>
     <cfRule type="duplicateValues" dxfId="142" priority="798"/>
-    <cfRule type="duplicateValues" dxfId="141" priority="797"/>
-    <cfRule type="duplicateValues" dxfId="140" priority="801"/>
-    <cfRule type="duplicateValues" dxfId="139" priority="800"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="799"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="800"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="801"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
-    <cfRule type="duplicateValues" dxfId="138" priority="795"/>
-    <cfRule type="duplicateValues" dxfId="137" priority="796"/>
-    <cfRule type="duplicateValues" dxfId="136" priority="792"/>
-    <cfRule type="duplicateValues" dxfId="135" priority="793"/>
-    <cfRule type="duplicateValues" dxfId="134" priority="794"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="792"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="793"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="794"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="795"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="796"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="duplicateValues" dxfId="133" priority="788"/>
-    <cfRule type="duplicateValues" dxfId="132" priority="789"/>
-    <cfRule type="duplicateValues" dxfId="131" priority="787"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="787"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="788"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="789"/>
     <cfRule type="duplicateValues" dxfId="130" priority="790"/>
     <cfRule type="duplicateValues" dxfId="129" priority="791"/>
   </conditionalFormatting>
@@ -8412,18 +8413,18 @@
     <cfRule type="duplicateValues" dxfId="119" priority="781"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A123">
-    <cfRule type="duplicateValues" dxfId="118" priority="776"/>
-    <cfRule type="duplicateValues" dxfId="117" priority="775"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="772"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="773"/>
     <cfRule type="duplicateValues" dxfId="116" priority="774"/>
-    <cfRule type="duplicateValues" dxfId="115" priority="773"/>
-    <cfRule type="duplicateValues" dxfId="114" priority="772"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="775"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="776"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126">
-    <cfRule type="duplicateValues" dxfId="113" priority="768"/>
-    <cfRule type="duplicateValues" dxfId="112" priority="771"/>
-    <cfRule type="duplicateValues" dxfId="111" priority="770"/>
-    <cfRule type="duplicateValues" dxfId="110" priority="769"/>
-    <cfRule type="duplicateValues" dxfId="109" priority="767"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="767"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="768"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="769"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="770"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="771"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A129">
     <cfRule type="duplicateValues" dxfId="108" priority="762"/>
@@ -8435,50 +8436,50 @@
   <conditionalFormatting sqref="A132">
     <cfRule type="duplicateValues" dxfId="103" priority="757"/>
     <cfRule type="duplicateValues" dxfId="102" priority="758"/>
-    <cfRule type="duplicateValues" dxfId="101" priority="760"/>
-    <cfRule type="duplicateValues" dxfId="100" priority="761"/>
-    <cfRule type="duplicateValues" dxfId="99" priority="759"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="759"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="760"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="761"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135">
     <cfRule type="duplicateValues" dxfId="98" priority="752"/>
-    <cfRule type="duplicateValues" dxfId="97" priority="754"/>
-    <cfRule type="duplicateValues" dxfId="96" priority="755"/>
-    <cfRule type="duplicateValues" dxfId="95" priority="756"/>
-    <cfRule type="duplicateValues" dxfId="94" priority="753"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="753"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="754"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="755"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="756"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="duplicateValues" dxfId="93" priority="751"/>
-    <cfRule type="duplicateValues" dxfId="92" priority="749"/>
-    <cfRule type="duplicateValues" dxfId="91" priority="748"/>
-    <cfRule type="duplicateValues" dxfId="90" priority="747"/>
-    <cfRule type="duplicateValues" dxfId="89" priority="750"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="747"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="748"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="749"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="750"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="751"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="88" priority="744"/>
-    <cfRule type="duplicateValues" dxfId="87" priority="746"/>
-    <cfRule type="duplicateValues" dxfId="86" priority="745"/>
-    <cfRule type="duplicateValues" dxfId="85" priority="743"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="742"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="742"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="743"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="744"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="745"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="746"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151">
     <cfRule type="duplicateValues" dxfId="83" priority="618"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
     <cfRule type="duplicateValues" dxfId="82" priority="737"/>
-    <cfRule type="duplicateValues" dxfId="81" priority="741"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="740"/>
-    <cfRule type="duplicateValues" dxfId="79" priority="739"/>
-    <cfRule type="duplicateValues" dxfId="78" priority="738"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="738"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="739"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="740"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="741"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A160">
     <cfRule type="duplicateValues" dxfId="77" priority="617"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A162">
-    <cfRule type="duplicateValues" dxfId="76" priority="734"/>
-    <cfRule type="duplicateValues" dxfId="75" priority="736"/>
-    <cfRule type="duplicateValues" dxfId="74" priority="735"/>
-    <cfRule type="duplicateValues" dxfId="73" priority="733"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="732"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="732"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="733"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="734"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="735"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="736"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A170">
     <cfRule type="duplicateValues" dxfId="71" priority="727"/>
@@ -8488,102 +8489,372 @@
     <cfRule type="duplicateValues" dxfId="67" priority="731"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A178">
-    <cfRule type="duplicateValues" dxfId="66" priority="726"/>
-    <cfRule type="duplicateValues" dxfId="65" priority="725"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="722"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="723"/>
     <cfRule type="duplicateValues" dxfId="64" priority="724"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="723"/>
-    <cfRule type="duplicateValues" dxfId="62" priority="722"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="725"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="726"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A184">
-    <cfRule type="duplicateValues" dxfId="61" priority="719"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="721"/>
-    <cfRule type="duplicateValues" dxfId="59" priority="720"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="718"/>
-    <cfRule type="duplicateValues" dxfId="57" priority="717"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="717"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="718"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="719"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="720"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="721"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A190">
-    <cfRule type="duplicateValues" dxfId="56" priority="714"/>
-    <cfRule type="duplicateValues" dxfId="55" priority="715"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="716"/>
-    <cfRule type="duplicateValues" dxfId="53" priority="713"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="712"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="712"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="713"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="714"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="715"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="716"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A193">
     <cfRule type="duplicateValues" dxfId="51" priority="707"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="711"/>
-    <cfRule type="duplicateValues" dxfId="49" priority="710"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="709"/>
-    <cfRule type="duplicateValues" dxfId="47" priority="708"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="708"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="709"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="710"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="711"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A197">
-    <cfRule type="duplicateValues" dxfId="46" priority="706"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="705"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="702"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="703"/>
     <cfRule type="duplicateValues" dxfId="44" priority="704"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="703"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="702"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="705"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="706"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A204">
-    <cfRule type="duplicateValues" dxfId="41" priority="698"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="699"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="697"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="701"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="700"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="697"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="698"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="699"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="700"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="701"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A211">
     <cfRule type="duplicateValues" dxfId="36" priority="692"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="696"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="695"/>
-    <cfRule type="duplicateValues" dxfId="33" priority="694"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="693"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="693"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="694"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="695"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="696"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A218">
-    <cfRule type="duplicateValues" dxfId="31" priority="691"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="689"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="688"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="687"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="690"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="687"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="688"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="689"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="690"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="691"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220">
-    <cfRule type="duplicateValues" dxfId="26" priority="685"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="684"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="686"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="683"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="682"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="682"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="683"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="684"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="685"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="686"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A231">
     <cfRule type="duplicateValues" dxfId="21" priority="677"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="681"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="680"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="679"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="678"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="678"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="679"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="680"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="681"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A238:A244">
     <cfRule type="duplicateValues" dxfId="16" priority="919"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A247">
-    <cfRule type="duplicateValues" dxfId="15" priority="889"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="887"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="888"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="887"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="888"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="889"/>
     <cfRule type="duplicateValues" dxfId="12" priority="890"/>
     <cfRule type="duplicateValues" dxfId="11" priority="917"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A255">
-    <cfRule type="duplicateValues" dxfId="10" priority="883"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="884"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="885"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="886"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="882"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="882"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="883"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="884"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="885"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="886"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261">
     <cfRule type="duplicateValues" dxfId="5" priority="877"/>
     <cfRule type="duplicateValues" dxfId="4" priority="878"/>
     <cfRule type="duplicateValues" dxfId="3" priority="879"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="881"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="880"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="880"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="881"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D7">
     <cfRule type="duplicateValues" dxfId="0" priority="598"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EED6D3-8290-440E-A4B4-BCAA5F91DE67}">
+  <dimension ref="B2:D52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>